<commit_message>
Used macro to generate new col for timeSpent (on problem)
</commit_message>
<xml_diff>
--- a/Leetcode Solution Tracker Sheet.xlsx
+++ b/Leetcode Solution Tracker Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mykel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PeiRu\OneDrive\桌面\999\VS CODE\1337\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE5B3E-E2E0-4865-B777-F7802F2B9769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D47C0C-69F1-40C2-91F6-B07FCB742A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="2070" windowWidth="21600" windowHeight="11325" xr2:uid="{81E507EF-14CC-4729-BA88-308D95D3D809}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{81E507EF-14CC-4729-BA88-308D95D3D809}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="23" r:id="rId1"/>
@@ -41,21 +41,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="198">
   <si>
     <t>Each sheet of this spreadsheet contains a leetcode pattern. While these questions aren't an exhaustive list of all leetcode questions, if you are able to  go through these questions with relative ease, most leetode questions should come relatively easy for you.</t>
   </si>
@@ -1071,95 +1062,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE07CE-C5DC-42F8-BD16-06E5A44770B0}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="242.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="242.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>190</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>191</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>192</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>193</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>194</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>196</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>197</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
@@ -1175,25 +1167,26 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DA2DE4-55DF-43CF-A5CF-2A414F185168}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1228,7 +1221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -1261,7 +1254,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>876</v>
       </c>
@@ -1272,7 +1265,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>234</v>
       </c>
@@ -1283,7 +1276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>203</v>
       </c>
@@ -1294,7 +1287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>83</v>
       </c>
@@ -1305,7 +1298,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>142</v>
       </c>
@@ -1316,7 +1309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2</v>
       </c>
@@ -1327,7 +1320,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>19</v>
       </c>
@@ -1338,7 +1331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>148</v>
       </c>
@@ -1349,7 +1342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>143</v>
       </c>
@@ -1367,25 +1360,26 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32BF07F-8940-4D2C-A939-C2AFCD4748B7}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1420,7 +1414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -1453,7 +1447,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>261</v>
       </c>
@@ -1464,7 +1458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>323</v>
       </c>
@@ -1475,7 +1469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>207</v>
       </c>
@@ -1486,7 +1480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>210</v>
       </c>
@@ -1497,7 +1491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>310</v>
       </c>
@@ -1508,7 +1502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>444</v>
       </c>
@@ -1519,7 +1513,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>269</v>
       </c>
@@ -1530,7 +1524,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1203</v>
       </c>
@@ -1548,25 +1542,26 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD685EA-FF73-4C9A-B882-70663E9C48A2}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1601,7 +1596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -1634,7 +1629,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>621</v>
       </c>
@@ -1645,7 +1640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>452</v>
       </c>
@@ -1656,7 +1651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>767</v>
       </c>
@@ -1667,7 +1662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>759</v>
       </c>
@@ -1678,7 +1673,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>358</v>
       </c>
@@ -1689,7 +1684,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>630</v>
       </c>
@@ -1707,25 +1702,26 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0C640-B452-44FE-8DC8-B3CA1F450589}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1760,7 +1756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -1793,7 +1789,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>373</v>
       </c>
@@ -1804,7 +1800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>253</v>
       </c>
@@ -1815,7 +1811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>621</v>
       </c>
@@ -1826,7 +1822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>973</v>
       </c>
@@ -1837,7 +1833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>347</v>
       </c>
@@ -1848,7 +1844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>451</v>
       </c>
@@ -1859,7 +1855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>215</v>
       </c>
@@ -1870,7 +1866,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>767</v>
       </c>
@@ -1881,7 +1877,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>23</v>
       </c>
@@ -1892,7 +1888,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>632</v>
       </c>
@@ -1903,7 +1899,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>759</v>
       </c>
@@ -1914,7 +1910,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>358</v>
       </c>
@@ -1925,7 +1921,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>630</v>
       </c>
@@ -1936,7 +1932,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>895</v>
       </c>
@@ -1947,7 +1943,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>295</v>
       </c>
@@ -1958,7 +1954,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>480</v>
       </c>
@@ -1976,25 +1972,26 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654C522A-ED9A-4FAE-A1D0-A2AEDBF5A3DA}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2029,7 +2026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -2062,7 +2059,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>92</v>
       </c>
@@ -2073,7 +2070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>61</v>
       </c>
@@ -2084,7 +2081,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>24</v>
       </c>
@@ -2095,7 +2092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>328</v>
       </c>
@@ -2106,7 +2103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>25</v>
       </c>
@@ -2124,25 +2121,26 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD8C66D-E592-4F8B-BCB3-70AC88A5C829}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2177,7 +2175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -2210,7 +2208,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>56</v>
       </c>
@@ -2221,7 +2219,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>986</v>
       </c>
@@ -2232,7 +2230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>435</v>
       </c>
@@ -2243,7 +2241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>253</v>
       </c>
@@ -2254,7 +2252,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>57</v>
       </c>
@@ -2269,25 +2267,26 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20EC155-3091-4863-8F61-30B4AD6E7C18}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2322,7 +2321,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>904</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>567</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>424</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -2399,7 +2398,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>239</v>
       </c>
@@ -2410,7 +2409,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>995</v>
       </c>
@@ -2421,7 +2420,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>828</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>76</v>
       </c>
@@ -2443,7 +2442,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>30</v>
       </c>
@@ -2461,25 +2460,26 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5CAA95-173A-4AAB-9830-51CFE57AFDA9}">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -2554,25 +2554,26 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CEE56F-7E6D-404D-A515-4BE4543A52FB}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2607,7 +2608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>210</v>
       </c>
@@ -2651,7 +2652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>310</v>
       </c>
@@ -2662,7 +2663,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>444</v>
       </c>
@@ -2673,7 +2674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>269</v>
       </c>
@@ -2684,7 +2685,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1203</v>
       </c>
@@ -2702,25 +2703,26 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC107CF8-8FA5-45A4-A6AC-1F5EF6ACED14}">
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2755,7 +2757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -2788,7 +2790,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1065</v>
       </c>
@@ -2799,7 +2801,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>208</v>
       </c>
@@ -2810,7 +2812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>421</v>
       </c>
@@ -2821,7 +2823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>212</v>
       </c>
@@ -2832,7 +2834,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>472</v>
       </c>
@@ -2843,7 +2845,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>745</v>
       </c>
@@ -2854,7 +2856,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>336</v>
       </c>
@@ -2865,7 +2867,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>425</v>
       </c>
@@ -2876,7 +2878,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>642</v>
       </c>
@@ -2894,25 +2896,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CCFF23-1D10-486A-BEF9-7C7E811BBE63}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2947,7 +2950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3">
         <v>111</v>
@@ -2996,7 +2999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>133</v>
       </c>
@@ -3011,7 +3014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>417</v>
       </c>
@@ -3026,7 +3029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>238</v>
       </c>
@@ -3041,7 +3044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>200</v>
       </c>
@@ -3056,7 +3059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>261</v>
       </c>
@@ -3071,7 +3074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>323</v>
       </c>
@@ -3086,7 +3089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>207</v>
       </c>
@@ -3101,7 +3104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>210</v>
       </c>
@@ -3116,7 +3119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>310</v>
       </c>
@@ -3131,7 +3134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>107</v>
       </c>
@@ -3146,7 +3149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>102</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>103</v>
       </c>
@@ -3176,7 +3179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>116</v>
       </c>
@@ -3191,7 +3194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>117</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>199</v>
       </c>
@@ -3221,7 +3224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>863</v>
       </c>
@@ -3243,25 +3246,26 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED98FAFF-47C9-43F7-9B0F-59BE26161DDA}">
+  <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3296,7 +3300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -3329,7 +3333,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -3340,7 +3344,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>977</v>
       </c>
@@ -3351,7 +3355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>844</v>
       </c>
@@ -3362,7 +3366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>287</v>
       </c>
@@ -3373,7 +3377,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>15</v>
       </c>
@@ -3384,7 +3388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>16</v>
       </c>
@@ -3395,7 +3399,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>713</v>
       </c>
@@ -3406,7 +3410,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>75</v>
       </c>
@@ -3417,7 +3421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>11</v>
       </c>
@@ -3428,7 +3432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>42</v>
       </c>
@@ -3446,25 +3450,26 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8ADC86-895E-43D9-BBDD-49D046E5BE81}">
+  <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3499,7 +3504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -3532,7 +3537,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>261</v>
       </c>
@@ -3543,7 +3548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>323</v>
       </c>
@@ -3561,25 +3566,26 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62E5DD5-98CB-43EF-B0C5-4D268FDD1BB7}">
+  <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3614,7 +3620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -3647,7 +3653,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>268</v>
       </c>
@@ -3658,7 +3664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>448</v>
       </c>
@@ -3669,7 +3675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>136</v>
       </c>
@@ -3680,7 +3686,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>238</v>
       </c>
@@ -3691,7 +3697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>287</v>
       </c>
@@ -3702,7 +3708,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>442</v>
       </c>
@@ -3713,7 +3719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>73</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>54</v>
       </c>
@@ -3735,7 +3741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>48</v>
       </c>
@@ -3746,7 +3752,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>41</v>
       </c>
@@ -3757,7 +3763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>128</v>
       </c>
@@ -3775,25 +3781,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D32482C-F28D-40F8-B266-25BFECB4E7E2}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3828,7 +3835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -3861,7 +3868,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>784</v>
       </c>
@@ -3872,7 +3879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>78</v>
       </c>
@@ -3883,7 +3890,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>90</v>
       </c>
@@ -3894,7 +3901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>46</v>
       </c>
@@ -3905,7 +3912,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>47</v>
       </c>
@@ -3916,7 +3923,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>77</v>
       </c>
@@ -3927,7 +3934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>39</v>
       </c>
@@ -3938,7 +3945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>40</v>
       </c>
@@ -3949,7 +3956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>216</v>
       </c>
@@ -3960,7 +3967,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>22</v>
       </c>
@@ -3971,7 +3978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>131</v>
       </c>
@@ -3982,7 +3989,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>17</v>
       </c>
@@ -3993,7 +4000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>320</v>
       </c>
@@ -4004,7 +4011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>37</v>
       </c>
@@ -4015,7 +4022,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>51</v>
       </c>
@@ -4033,25 +4040,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E22EEC-C94F-4CDA-B6C9-E056366EC292}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4086,7 +4094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -4119,7 +4127,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>744</v>
       </c>
@@ -4130,7 +4138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>852</v>
       </c>
@@ -4141,7 +4149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>287</v>
       </c>
@@ -4152,7 +4160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>378</v>
       </c>
@@ -4163,7 +4171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>153</v>
       </c>
@@ -4174,7 +4182,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>162</v>
       </c>
@@ -4185,7 +4193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>33</v>
       </c>
@@ -4196,7 +4204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>81</v>
       </c>
@@ -4207,7 +4215,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>74</v>
       </c>
@@ -4218,7 +4226,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>240</v>
       </c>
@@ -4229,7 +4237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>658</v>
       </c>
@@ -4240,7 +4248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>327</v>
       </c>
@@ -4251,7 +4259,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>4</v>
       </c>
@@ -4269,25 +4277,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{775ED7CA-6A81-4468-B9F1-B5D1BC69F03A}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4322,7 +4331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -4355,7 +4364,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>136</v>
       </c>
@@ -4373,25 +4382,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0539E18-BFA6-4FC5-BB15-87D35B593DB4}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4426,7 +4436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -4466,25 +4476,26 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A096B0B-54F9-4AF8-9FF2-51932738441C}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4519,7 +4530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -4552,7 +4563,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>100</v>
       </c>
@@ -4563,7 +4574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>112</v>
       </c>
@@ -4574,7 +4585,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>543</v>
       </c>
@@ -4585,7 +4596,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>617</v>
       </c>
@@ -4596,7 +4607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>104</v>
       </c>
@@ -4607,7 +4618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>235</v>
       </c>
@@ -4618,7 +4629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>572</v>
       </c>
@@ -4629,7 +4640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>226</v>
       </c>
@@ -4640,7 +4651,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>494</v>
       </c>
@@ -4651,7 +4662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>133</v>
       </c>
@@ -4662,7 +4673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>417</v>
       </c>
@@ -4673,7 +4684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>200</v>
       </c>
@@ -4684,7 +4695,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -4692,7 +4703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>200</v>
       </c>
@@ -4703,7 +4714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>23</v>
       </c>
@@ -4711,7 +4722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>230</v>
       </c>
@@ -4722,7 +4733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>207</v>
       </c>
@@ -4733,7 +4744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>210</v>
       </c>
@@ -4744,7 +4755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>199</v>
       </c>
@@ -4755,7 +4766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>863</v>
       </c>
@@ -4766,7 +4777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>113</v>
       </c>
@@ -4777,7 +4788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>437</v>
       </c>
@@ -4788,7 +4799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>236</v>
       </c>
@@ -4799,7 +4810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>654</v>
       </c>
@@ -4810,7 +4821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>662</v>
       </c>
@@ -4821,7 +4832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>105</v>
       </c>
@@ -4832,7 +4843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>98</v>
       </c>
@@ -4843,7 +4854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>124</v>
       </c>
@@ -4854,7 +4865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>212</v>
       </c>
@@ -4865,7 +4876,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>1203</v>
       </c>
@@ -4883,25 +4894,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C665F7-2A47-4849-9374-5FC3BE7713BB}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4936,7 +4948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44340</v>
       </c>
@@ -4969,7 +4981,7 @@
         <v>44403</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>297</v>
       </c>
@@ -4987,25 +4999,26 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE603ED-64B5-4F47-AFAA-7F85BFF19FBE}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5040,10 +5053,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>44340</v>
-      </c>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
       <c r="B2">
         <v>70</v>
       </c>
@@ -5053,27 +5064,24 @@
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" s="1">
         <f>DATE(YEAR(A2),MONTH(A2),DAY(A2) + IF(F2 = "Y", 14, 7))</f>
-        <v>44354</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1">
         <f>DATE(YEAR(G2),MONTH(G2),DAY(G2)+7)</f>
-        <v>44361</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1">
         <f>DATE(YEAR(H2),MONTH(H2),DAY(H2)+14)</f>
-        <v>44375</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1">
         <f>DATE(YEAR(I2),MONTH(I2),DAY(I2)+28)</f>
-        <v>44403</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>121</v>
       </c>
@@ -5084,7 +5092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>53</v>
       </c>
@@ -5095,7 +5103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>303</v>
       </c>
@@ -5106,7 +5114,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>494</v>
       </c>
@@ -5117,7 +5125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>198</v>
       </c>
@@ -5128,7 +5136,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>213</v>
       </c>
@@ -5139,7 +5147,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>322</v>
       </c>
@@ -5150,7 +5158,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>152</v>
       </c>
@@ -5161,7 +5169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>300</v>
       </c>
@@ -5172,7 +5180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>5</v>
       </c>
@@ -5183,7 +5191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>139</v>
       </c>
@@ -5194,7 +5202,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>377</v>
       </c>
@@ -5205,7 +5213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>91</v>
       </c>
@@ -5216,7 +5224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>62</v>
       </c>
@@ -5227,7 +5235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>55</v>
       </c>
@@ -5238,7 +5246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>647</v>
       </c>
@@ -5249,7 +5257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>673</v>
       </c>
@@ -5260,7 +5268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>416</v>
       </c>
@@ -5271,7 +5279,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>698</v>
       </c>
@@ -5282,7 +5290,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>309</v>
       </c>
@@ -5293,7 +5301,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>338</v>
       </c>

</xml_diff>